<commit_message>
new R package BioMathR
</commit_message>
<xml_diff>
--- a/CV/CVcontent.xlsx
+++ b/CV/CVcontent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Schmidtpaul.github.io\CV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSchmidt\Documents\GitHub\Schmidtpaul.github.io\CV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B3B224-44DF-4844-854A-059138B5EF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2984F3-0607-4318-8A66-FB63CF8169B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1050" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Job" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="149">
   <si>
     <t>BioMath - Applied Statistics and Informatics in Life Sciences</t>
   </si>
@@ -453,16 +453,22 @@
     <t xml:space="preserve">Website https://schmidtpaul.github.io/dsfair_quarto/ </t>
   </si>
   <si>
-    <t>R Paket CitaviR schmidtpaul.github.io/CitaviR/.</t>
-  </si>
-  <si>
-    <t>R package CitaviR https://schmidtpaul.github.io/CitaviR/.</t>
-  </si>
-  <si>
     <t>see 'Workshops' section below</t>
   </si>
   <si>
     <t>siehe 'Workshops' Abschnitt unten</t>
+  </si>
+  <si>
+    <t>R package BioMathR https://schmidtpaul.github.io/BioMathR/</t>
+  </si>
+  <si>
+    <t>R Paket BioMathR https://schmidtpaul.github.io/BioMathR/</t>
+  </si>
+  <si>
+    <t>R Paket CitaviR schmidtpaul.github.io/CitaviR/</t>
+  </si>
+  <si>
+    <t>R package CitaviR https://schmidtpaul.github.io/CitaviR/</t>
   </si>
 </sst>
 </file>
@@ -853,7 +859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -1063,10 +1069,10 @@
         <v>31</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>7</v>
@@ -1093,10 +1099,10 @@
         <v>31</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>8</v>
@@ -1691,11 +1697,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D89F78D-EC1A-4292-B5B7-FAB02BA43469}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1739,24 +1743,24 @@
         <v>125</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>92</v>
+        <v>148</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1767,10 +1771,10 @@
         <v>124</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1781,10 +1785,10 @@
         <v>124</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1795,10 +1799,10 @@
         <v>124</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1809,10 +1813,10 @@
         <v>124</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1823,24 +1827,24 @@
         <v>124</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1851,24 +1855,24 @@
         <v>126</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1879,10 +1883,10 @@
         <v>101</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1893,10 +1897,10 @@
         <v>101</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1907,10 +1911,10 @@
         <v>101</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1921,10 +1925,10 @@
         <v>101</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1935,10 +1939,10 @@
         <v>101</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1949,10 +1953,10 @@
         <v>101</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1963,10 +1967,10 @@
         <v>101</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1977,24 +1981,24 @@
         <v>101</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2005,10 +2009,10 @@
         <v>131</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2019,24 +2023,24 @@
         <v>131</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2047,10 +2051,10 @@
         <v>132</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2061,10 +2065,10 @@
         <v>132</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2075,9 +2079,23 @@
         <v>132</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>136</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cv & workshop update
</commit_message>
<xml_diff>
--- a/CV/CVcontent.xlsx
+++ b/CV/CVcontent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSchmidt\Documents\GitHub\Schmidtpaul.github.io\CV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2984F3-0607-4318-8A66-FB63CF8169B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223E6A13-C7C5-49E6-A688-698BBA14F546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1050" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Job" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="146">
   <si>
     <t>BioMath - Applied Statistics and Informatics in Life Sciences</t>
   </si>
@@ -30,18 +30,9 @@
     <t>Rostock &amp; Hamburg, Germany</t>
   </si>
   <si>
-    <t>Various statistical analyses from raw data to final report for e.g. yearly post-market monitoring (survey; agriculture), risk assessment (meta-analysis; epidemiology), a long-term field trial (experiment; environment), geographic distribution (geospatial; administrative office)</t>
-  </si>
-  <si>
     <t>Implement new / streamline existing SOPs (for e.g. systematic literature reviews and meta-analyses) by making better use of in-depth functionality of established software and additionally via introducing complementing software/tools</t>
   </si>
   <si>
-    <t>Supervise project communication and time management</t>
-  </si>
-  <si>
-    <t>Conduct in-depth research,  write scientific reports and proofread especially English tender application, report and publication drafts</t>
-  </si>
-  <si>
     <t>Freelancer (part-time)</t>
   </si>
   <si>
@@ -150,18 +141,9 @@
     <t>General manager since September 2022</t>
   </si>
   <si>
-    <t>Verschiedene statistische Analysen von Rohdaten bis zum Schlussbericht für z.B. jährliches post-market Monitoring (Umfrage; Landwirtschaft), Risikobewertung (Metaanalyse; Epidemiologie), mehrjähriger Feldversuche (Experiment; Umwelt), Geografische Verteilung (GIS; Landesamt)</t>
-  </si>
-  <si>
     <t>Implementierung neuer / Optimierung vorhandener SOPs (z.B. für systematic literature reviews und Metaanalysen), indem beispielsweise die Funktionalität vorhandener Software besser genutzt wird und zusätzlich ergänzende Software/Tools eingesetzt werden</t>
   </si>
   <si>
-    <t>Koordination der Kommunikation und des Zeitmanagements von Projekten</t>
-  </si>
-  <si>
-    <t>Durchführung von detaillierten Recherchen und Verfassen von wissenschaftlichen Texten</t>
-  </si>
-  <si>
     <t>Durchführung von Workshops zu Statistik mit R; der genaue Inhalt und die Kurssprache in Absprache mit dem Auftraggeber</t>
   </si>
   <si>
@@ -342,15 +324,6 @@
     <t>Python</t>
   </si>
   <si>
-    <t>MS Office</t>
-  </si>
-  <si>
-    <t>Adoce Acrobat Pro</t>
-  </si>
-  <si>
-    <t>Latex</t>
-  </si>
-  <si>
     <t>SQL</t>
   </si>
   <si>
@@ -435,9 +408,6 @@
     <t>Präsentationen</t>
   </si>
   <si>
-    <t>C#</t>
-  </si>
-  <si>
     <t>exploratory &amp; descriptive data analysis</t>
   </si>
   <si>
@@ -469,6 +439,27 @@
   </si>
   <si>
     <t>R package CitaviR https://schmidtpaul.github.io/CitaviR/</t>
+  </si>
+  <si>
+    <t>Conduct systematic reviews, write and proofread scientific reports</t>
+  </si>
+  <si>
+    <t>Durchführung von Systematic Reviews und Verfassen un Korrekturlesen von wissenschaftlichen Texten</t>
+  </si>
+  <si>
+    <t>MS Office (VBA)</t>
+  </si>
+  <si>
+    <t>Various statistical analyses from raw data to final report, including conceptualization of research approach; data acquisition, cleansing, and integration; data analysis and modeling; interpretation, presentation, and communication of results.</t>
+  </si>
+  <si>
+    <t>Recent projects: Time series and correlation analysis of air parameters; Comparison of agricultural treatments; Co-creation and evaluation of monitoring surveys; Epidemiological risk assessments using meta-analyses; Evaluation of geographical distributions using GIS data.</t>
+  </si>
+  <si>
+    <t>Verschiedene statistische Analysen von Rohdaten bis Schlussbericht, d.h. Konzeption der Herangehensweise an die Fragestellung; Beschaffung, Bereinigung und Zusammenführung von Daten; Analyse und Modellierung; Interpretation, Aufbereitung und Vermittlung der Ergebnisse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kürzliche Projekte: Zeitreihen- und Zusammenhangsanalysen von Luftparametern; Vergleich von landwirtschaftlichen Behandlungen; Konzeption und Auswertung von Monitorings; Epidemiologische Risikobewertungen via Meta-Analyse; Geografischen Verteilungen mit GIS-Daten </t>
   </si>
 </sst>
 </file>
@@ -859,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -871,34 +862,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -907,10 +898,10 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>0</v>
@@ -922,13 +913,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>2</v>
+        <v>142</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>42</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -937,10 +928,10 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>0</v>
@@ -952,13 +943,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -967,10 +958,10 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>0</v>
@@ -982,13 +973,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -997,10 +988,10 @@
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>0</v>
@@ -1012,13 +1003,13 @@
         <v>1</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>5</v>
+        <v>139</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>45</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1027,10 +1018,10 @@
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>0</v>
@@ -1042,13 +1033,13 @@
         <v>1</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1057,28 +1048,28 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1087,28 +1078,28 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1119,28 +1110,28 @@
         <v>43465</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="J9" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1151,28 +1142,28 @@
         <v>43465</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="J10" s="6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1183,28 +1174,28 @@
         <v>43465</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="J11" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1215,28 +1206,28 @@
         <v>43465</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1247,10 +1238,10 @@
         <v>42246</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>0</v>
@@ -1259,16 +1250,16 @@
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1279,10 +1270,10 @@
         <v>42246</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>0</v>
@@ -1291,16 +1282,16 @@
         <v>0</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1347,34 +1338,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1385,28 +1376,28 @@
         <v>43799</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1417,28 +1408,28 @@
         <v>43799</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1449,28 +1440,28 @@
         <v>42369</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="H4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="J4" s="6" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1481,28 +1472,28 @@
         <v>42369</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="H5" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1513,28 +1504,28 @@
         <v>42004</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1545,28 +1536,28 @@
         <v>42004</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1577,28 +1568,28 @@
         <v>41182</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1609,28 +1600,28 @@
         <v>41182</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1641,28 +1632,28 @@
         <v>39294</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1697,9 +1688,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D89F78D-EC1A-4292-B5B7-FAB02BA43469}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1709,254 +1700,254 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1964,13 +1955,13 @@
         <v>101</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1978,13 +1969,13 @@
         <v>101</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1992,111 +1983,69 @@
         <v>101</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>